<commit_message>
Arquivo final do projeto
</commit_message>
<xml_diff>
--- a/Leao_APP.xlsx
+++ b/Leao_APP.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2cfd62044dba754/Área de Trabalho/Excel - Santander/Imposto de Renda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2cfd62044dba754/Área de Trabalho/Excel - Santander/Imposto de Renda/app_income_tax/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="340" documentId="8_{F5E2AA90-17DE-4235-A42E-60D809282AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72528B22-8109-4DCB-9502-C562AB00EBDF}"/>
+  <xr:revisionPtr revIDLastSave="544" documentId="8_{F5E2AA90-17DE-4235-A42E-60D809282AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D8E3D6F-9D24-4550-9CE7-79DDE5F4D0FC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{65926913-E296-4B84-95EC-D96CED0EA6C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{65926913-E296-4B84-95EC-D96CED0EA6C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Titular" sheetId="1" r:id="rId1"/>
     <sheet name="Informes" sheetId="2" r:id="rId2"/>
     <sheet name="Notas" sheetId="3" r:id="rId3"/>
-    <sheet name="Tabelas" sheetId="4" r:id="rId4"/>
+    <sheet name="Tabelas" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>NOME</t>
   </si>
@@ -273,21 +273,64 @@
   </si>
   <si>
     <t>001 - Banco do Brasil</t>
+  </si>
+  <si>
+    <t>1º Banco</t>
+  </si>
+  <si>
+    <t>2º Banco</t>
+  </si>
+  <si>
+    <t>3º Banco</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Exercício</t>
+  </si>
+  <si>
+    <t>3. NOTAS / RECIBOS / HOLERITES</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>ENTRADAS</t>
+  </si>
+  <si>
+    <t>HOLERITE(CONTRA-CHEQUE)</t>
+  </si>
+  <si>
+    <t>NOTA FISCAL DE SERVIÇO</t>
+  </si>
+  <si>
+    <t>RECIBO</t>
+  </si>
+  <si>
+    <t>TOTAL RENDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
-    <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
-    <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;)&quot;0000&quot;-&quot;0000"/>
-    <numFmt numFmtId="167" formatCode="&quot;(&quot;00&quot;)&quot;0\ 0000&quot;-&quot;0000"/>
-    <numFmt numFmtId="168" formatCode="00&quot;.&quot;000&quot;-&quot;000"/>
-    <numFmt numFmtId="169" formatCode="0000&quot; &quot;0000&quot; &quot;0000"/>
-    <numFmt numFmtId="170" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
+    <numFmt numFmtId="165" formatCode="&quot;(&quot;00&quot;)&quot;0000&quot;-&quot;0000"/>
+    <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;)&quot;0\ 0000&quot;-&quot;0000"/>
+    <numFmt numFmtId="167" formatCode="00&quot;.&quot;000&quot;-&quot;000"/>
+    <numFmt numFmtId="168" formatCode="0000&quot; &quot;0000&quot; &quot;0000"/>
+    <numFmt numFmtId="169" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="172" formatCode="mmmm/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,8 +387,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,59 +519,205 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="4"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -500,13 +745,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>426384</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>170037</xdr:rowOff>
+      <xdr:rowOff>84312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2097741</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>171717</xdr:rowOff>
+      <xdr:rowOff>85992</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -567,7 +812,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>2505075</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>140635</xdr:rowOff>
+      <xdr:rowOff>54910</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -690,14 +935,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>169489</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>44825</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>168650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2365489</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>195001</xdr:rowOff>
+      <xdr:rowOff>109276</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -780,14 +1025,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>115981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2410312</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>15706</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>120481</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -863,13 +1108,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>184054</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>208429</xdr:rowOff>
+      <xdr:rowOff>122704</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2380054</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>145694</xdr:rowOff>
+      <xdr:rowOff>59969</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1130,13 +1375,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>56030</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:rowOff>3922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>302559</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:rowOff>93569</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1192,8 +1437,71 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>PRÓXIMO</a:t>
+            <a:t>PRÓXIMO </a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2105025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2571750</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta: para a Direita 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFB405E7-EE38-58D1-07E8-4DE4036F7A5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191500" y="4581525"/>
+          <a:ext cx="466725" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1215,7 +1523,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>2097741</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>48452</xdr:rowOff>
+      <xdr:rowOff>26041</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1400,13 +1708,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>169489</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>156883</xdr:rowOff>
+      <xdr:rowOff>112060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2365489</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>161383</xdr:rowOff>
+      <xdr:rowOff>94148</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1472,14 +1780,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2410312</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>71735</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82941</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1554,14 +1862,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>184054</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6723</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2380054</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>11223</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>89665</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1881,6 +2189,280 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247090</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo: Cantos Arredondados 8">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1BEC4F-1D69-411F-A44B-1C5BC74DFDF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6219265" y="5266765"/>
+          <a:ext cx="3227854" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="001E60"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>PRÓXIMO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>392205</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3014942</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo: Cantos Arredondados 9">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B497A082-7F24-4802-90B3-984B83E8082B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2902323" y="5266765"/>
+          <a:ext cx="3227854" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="001E60"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ANTERIOR	</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2084294</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2551019</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>128308</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Seta: para a Direita 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCCC90DB-1741-411D-A170-27F1D27A832A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8303559" y="5423648"/>
+          <a:ext cx="466725" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>376518</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>163606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>843243</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>135031</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Seta: para a Direita 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F8E8E07-A3BB-4234-8757-85D857C439E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3491753" y="5430371"/>
+          <a:ext cx="466725" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1890,14 +2472,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>426384</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>35566</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>170037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2097741</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>182923</xdr:rowOff>
+      <xdr:rowOff>48452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1957,8 +2539,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2505075</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>6164</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>140635</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2081,14 +2663,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>169489</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>100854</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2365489</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>105354</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161383</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2154,14 +2736,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2410312</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>15706</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>71735</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2253,13 +2835,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>184054</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>141194</xdr:rowOff>
+      <xdr:rowOff>6723</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2380054</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>145694</xdr:rowOff>
+      <xdr:rowOff>11223</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2419,13 +3001,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2353236</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2515,11 +3097,208 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 1" descr="Resultado de imagem para LIKEDIN ICONE">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0B0A414-7B79-4696-8F5C-DC639D08BF45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3124200" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>605116</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>672353</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Retângulo: Cantos Arredondados 10">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4069DE73-31C9-45AF-8346-499B51672221}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3115234" y="1064559"/>
+          <a:ext cx="1972237" cy="190499"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="001E60"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ANTERIOR	</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Seta: para a Direita 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31792C16-DFAC-42E5-B083-AE8275277B51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3272118" y="1086971"/>
+          <a:ext cx="347382" cy="134470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{20406D3E-9CC7-4EC3-9568-DC811A3F0EDF}" name="Tabela2" displayName="Tabela2" ref="C10:E34" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
+  <autoFilter ref="C10:E34" xr:uid="{20406D3E-9CC7-4EC3-9568-DC811A3F0EDF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A2404B44-F981-4A26-9581-133EA56FB452}" name="DATA" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9CD0489E-017B-4071-BC02-F2D854AFAD13}" name="CATEGORIA" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1BE5E3CA-3277-4C86-9EBF-8C4D140F2A76}" name="VALOR" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2842,8 +3621,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D8"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2853,138 +3632,146 @@
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
+      <c r="D2" s="31">
+        <v>2025</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="18">
         <v>45269806470</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="19">
         <v>29433</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="20">
         <v>338589659</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="21">
         <v>52120000</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="22">
         <v>813366958</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="23">
         <v>81996885632</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="24" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="24" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="24" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C4:E4"/>
   </mergeCells>
@@ -3001,10 +3788,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F245FF-A214-451B-A1EF-1658FBD6DF20}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,53 +3801,137 @@
     <col min="4" max="4" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
+      <c r="D2" s="12">
+        <f>Titular!$D$2</f>
+        <v>2025</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6" t="s">
+      <c r="C4" s="7" t="str">
+        <f>"Preencha os saldos das contas bancárias em 31/12/"&amp;Titular!$D$2</f>
+        <v>Preencha os saldos das contas bancárias em 31/12/2025</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <f>SUM(D12,D17,D22)</f>
+        <v>12726</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D11" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D12" s="25">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="25">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="26"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="25">
+        <v>8658</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C8:E8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -3068,7 +3939,7 @@
           <x14:formula1>
             <xm:f>Tabelas!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>D6</xm:sqref>
+          <xm:sqref>D11 D16 D21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3079,29 +3950,235 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDB6F30-EF21-4A72-B151-EDA84B09F399}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="E32:F33"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D2" s="12">
+        <f>Titular!$D$2</f>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="str">
+        <f>"Anexe os documentos de comprovação de entradas em "&amp;Titular!$D$2</f>
+        <v>Anexe os documentos de comprovação de entradas em 2025</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <f>SUM(Tabela2[VALOR])</f>
+        <v>5600</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="27">
+        <v>45962</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="29">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="27">
+        <v>45963</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="29">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="27">
+        <v>45964</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="30"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="30"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="30"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="30"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="30"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="30"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="30"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="30"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="30"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="30"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="30"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="30"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="30"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="30"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="30"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="29"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="30"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="30"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="29"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D34" xr:uid="{E8D59845-4597-4935-B3F7-E91E2044BEF8}">
+      <formula1>"HOLERITE(CONTRA-CHEQUE), NOTA FISCAL DE SERVIÇO, RECIBO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3119,7 +4196,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>